<commit_message>
Changes to grid aesthetic and other changes.
</commit_message>
<xml_diff>
--- a/Classes.xlsx
+++ b/Classes.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB81878-C512-4704-9483-220990FF9457}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Executioner" sheetId="1" r:id="rId1"/>
+    <sheet name="Squire" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,11 +20,74 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>Executioner</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Terminus Est</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Abilities</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Shroud</t>
+  </si>
+  <si>
+    <t>Become undetectable for 3 turns.</t>
+  </si>
+  <si>
+    <t>Kill any humanoid enemy under 50% HP.</t>
+  </si>
+  <si>
+    <t>Slow moving, resistant to CC, high melee damage.</t>
+  </si>
+  <si>
+    <t>Squire</t>
+  </si>
+  <si>
+    <t>High mobility, low HP, can use inventory, possibly support (depending on game mechanics, like armor).</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -37,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +110,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +409,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976B894A-ABB4-42E1-B09C-EEE54C6983D9}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>